<commit_message>
Pushing Queue and Graph module
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserRegistrationData.xlsx
+++ b/src/test/resources/testdata/UserRegistrationData.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14377\eclipse-workspace\numpy_ninja_ds_algo\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1168BE-7604-437A-934F-D2765D532A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{213E3FD9-CABD-4B62-8A59-AFA12BD5419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="signin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -545,10 +541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783ADBE4-C79C-4E77-B0BA-FFD759FD072B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +609,7 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Pushing Queue and Graph module"
This reverts commit 86fe86e253897326f76093de26d4f747dc7cf5ac.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserRegistrationData.xlsx
+++ b/src/test/resources/testdata/UserRegistrationData.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{213E3FD9-CABD-4B62-8A59-AFA12BD5419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14377\eclipse-workspace\numpy_ninja_ds_algo\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1168BE-7604-437A-934F-D2765D532A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="signin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -541,10 +545,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783ADBE4-C79C-4E77-B0BA-FFD759FD072B}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +613,6 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Revert "Pushing Queue and Graph module""
This reverts commit 6c7e5a2d935038d7d9908008791c46252549af39.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/UserRegistrationData.xlsx
+++ b/src/test/resources/testdata/UserRegistrationData.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14377\eclipse-workspace\numpy_ninja_ds_algo\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F1168BE-7604-437A-934F-D2765D532A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{213E3FD9-CABD-4B62-8A59-AFA12BD5419D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DAA46405-1568-4D3D-9B09-5FCA782EBB91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="signin" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -545,10 +541,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783ADBE4-C79C-4E77-B0BA-FFD759FD072B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,6 +609,7 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>